<commit_message>
Fix question’s answer selection upon next. Verify two corrects in a row work for same answer. Verify MA questions work Fix uploading bar issue. Change 1 2 3 4 MA to A B C D Remove Grunt Errors Ensure Row 1 xslx matches questions file to prevent incorrect upload. Check for duplicates for questions -doesn’t compare question Hint after 1st attempt URLs open in new tab
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\Biotility\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="25875" windowHeight="11760"/>
   </bookViews>
@@ -589,9 +594,6 @@
   </si>
   <si>
     <t>Most ATP in eukaryotic cells is produced in the:</t>
-  </si>
-  <si>
-    <t>Miotochondria</t>
   </si>
   <si>
     <t>Rough endoplasmic reticulum</t>
@@ -2049,6 +2051,9 @@
   </si>
   <si>
     <t>http://www.bioprocessintl.com/analytical/product-characterization/building-a-robust-bioassay-for-product-potency-measurement/</t>
+  </si>
+  <si>
+    <t>Mitochondria</t>
   </si>
 </sst>
 </file>
@@ -2781,6 +2786,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3114,8 +3122,8 @@
   <dimension ref="A1:AA280"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,19 +3185,19 @@
         <v>6</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>140</v>
-      </c>
       <c r="N1" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>49</v>
@@ -3233,7 +3241,7 @@
     </row>
     <row r="2" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>19</v>
@@ -3245,7 +3253,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>132</v>
+        <v>383</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>23</v>
@@ -3254,10 +3262,10 @@
         <v>24</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -3265,10 +3273,10 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
@@ -3682,40 +3690,40 @@
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="M11" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
@@ -3737,41 +3745,41 @@
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="I12" s="5" t="s">
+      <c r="L12" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="O12" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
@@ -3794,22 +3802,22 @@
         <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" s="5">
         <v>4</v>
       </c>
       <c r="E13" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>194</v>
-      </c>
       <c r="H13" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -3818,10 +3826,10 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
@@ -3843,22 +3851,22 @@
         <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" s="5">
         <v>2</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="G14" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>202</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -3867,10 +3875,10 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="P14" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
@@ -3892,22 +3900,22 @@
         <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -3916,10 +3924,10 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
@@ -3941,22 +3949,22 @@
         <v>19</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D16" s="5">
         <v>3</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -3965,10 +3973,10 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
@@ -3990,10 +3998,10 @@
         <v>20</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -4006,10 +4014,10 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
@@ -4031,7 +4039,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>21</v>
@@ -4047,10 +4055,10 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
@@ -4072,7 +4080,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>21</v>
@@ -4088,10 +4096,10 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
@@ -4113,10 +4121,10 @@
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -4129,10 +4137,10 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
@@ -4203,23 +4211,23 @@
         <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="J22" s="5">
         <v>2</v>
@@ -4237,10 +4245,10 @@
         <v>3</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
@@ -4262,7 +4270,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>21</v>
@@ -4278,10 +4286,10 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
@@ -4303,25 +4311,25 @@
         <v>18</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D24" s="5">
         <v>4</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="G24" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>360</v>
-      </c>
       <c r="I24" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -4329,10 +4337,10 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
@@ -4354,7 +4362,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D25" s="5">
         <v>3</v>
@@ -4369,10 +4377,10 @@
         <v>99</v>
       </c>
       <c r="H25" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>363</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>364</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -4380,10 +4388,10 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
@@ -4405,7 +4413,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D26" s="5">
         <v>2</v>
@@ -4420,10 +4428,10 @@
         <v>99</v>
       </c>
       <c r="H26" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="I26" s="5" t="s">
         <v>363</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>364</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -4431,10 +4439,10 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
@@ -4456,7 +4464,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D27" s="5">
         <v>5</v>
@@ -4471,10 +4479,10 @@
         <v>99</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>363</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>364</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -4482,10 +4490,10 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
@@ -4507,7 +4515,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>21</v>
@@ -4523,10 +4531,10 @@
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
@@ -4548,22 +4556,22 @@
         <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D29" s="5">
         <v>4</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="G29" s="4" t="s">
-        <v>377</v>
-      </c>
       <c r="H29" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -4572,10 +4580,10 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="P29" s="7" t="s">
         <v>380</v>
-      </c>
-      <c r="P29" s="7" t="s">
-        <v>381</v>
       </c>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
@@ -4597,10 +4605,10 @@
         <v>20</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>326</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -4613,10 +4621,10 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="P30" s="7" t="s">
         <v>330</v>
-      </c>
-      <c r="P30" s="7" t="s">
-        <v>331</v>
       </c>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
@@ -4638,7 +4646,7 @@
         <v>20</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>21</v>
@@ -4654,10 +4662,10 @@
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
@@ -4679,7 +4687,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>21</v>
@@ -4695,10 +4703,10 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
@@ -4720,10 +4728,10 @@
         <v>20</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -4736,10 +4744,10 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
@@ -4761,7 +4769,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>21</v>
@@ -4777,10 +4785,10 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="P34" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
@@ -4900,20 +4908,20 @@
         <v>18</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>269</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4">
@@ -4930,10 +4938,10 @@
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P37" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
@@ -5102,36 +5110,36 @@
         <v>18</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K41" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="L41" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P41" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
@@ -5153,37 +5161,37 @@
         <v>18</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F42" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K42" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L42" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="L42" s="4" t="s">
+      <c r="M42" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="M42" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="N42" s="4"/>
       <c r="O42" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
@@ -5206,36 +5214,36 @@
         <v>18</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="L43" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P43" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
@@ -5257,40 +5265,40 @@
         <v>18</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="H44" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="L44" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="M44" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="L44" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="N44" s="5"/>
       <c r="O44" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P44" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
@@ -5306,28 +5314,28 @@
     </row>
     <row r="45" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D45" s="5">
         <v>1</v>
       </c>
       <c r="E45" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="G45" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="G45" s="5" t="s">
+      <c r="H45" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
@@ -5336,10 +5344,10 @@
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P45" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
@@ -5355,28 +5363,28 @@
     </row>
     <row r="46" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D46" s="5">
         <v>4</v>
       </c>
       <c r="E46" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="G46" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>224</v>
-      </c>
       <c r="H46" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
@@ -5385,10 +5393,10 @@
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P46" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
@@ -5404,28 +5412,28 @@
     </row>
     <row r="47" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D47" s="5">
         <v>2</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F47" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="H47" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
@@ -5434,10 +5442,10 @@
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="O47" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P47" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="P47" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
@@ -5453,28 +5461,28 @@
     </row>
     <row r="48" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D48" s="5">
         <v>3</v>
       </c>
       <c r="E48" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="G48" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="H48" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
@@ -5483,10 +5491,10 @@
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="O48" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P48" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="P48" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="Q48" s="5"/>
       <c r="R48" s="5"/>
@@ -5502,28 +5510,28 @@
     </row>
     <row r="49" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
@@ -5532,10 +5540,10 @@
       <c r="M49" s="5"/>
       <c r="N49" s="5"/>
       <c r="O49" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P49" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="P49" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
@@ -5551,28 +5559,28 @@
     </row>
     <row r="50" spans="1:27" ht="45" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D50" s="5">
         <v>4</v>
       </c>
       <c r="E50" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="G50" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="G50" s="5" t="s">
+      <c r="H50" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
@@ -5581,10 +5589,10 @@
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P50" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="P50" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="Q50" s="5"/>
       <c r="R50" s="5"/>
@@ -5600,28 +5608,28 @@
     </row>
     <row r="51" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D51" s="5">
         <v>2</v>
       </c>
       <c r="E51" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="G51" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="G51" s="5" t="s">
+      <c r="H51" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
@@ -5630,10 +5638,10 @@
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P51" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="P51" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="Q51" s="5"/>
       <c r="R51" s="5"/>
@@ -5649,28 +5657,28 @@
     </row>
     <row r="52" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D52" s="5">
         <v>3</v>
       </c>
       <c r="E52" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="G52" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
@@ -5679,10 +5687,10 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P52" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="P52" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="Q52" s="5"/>
       <c r="R52" s="5"/>
@@ -5698,28 +5706,28 @@
     </row>
     <row r="53" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D53" s="5">
         <v>4</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
@@ -5728,10 +5736,10 @@
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
       <c r="O53" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P53" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="P53" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="Q53" s="5"/>
       <c r="R53" s="5"/>
@@ -5747,28 +5755,28 @@
     </row>
     <row r="54" spans="1:27" ht="66" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D54" s="5">
         <v>4</v>
       </c>
       <c r="E54" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="G54" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="G54" s="5" t="s">
-        <v>263</v>
-      </c>
       <c r="H54" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
@@ -5777,10 +5785,10 @@
       <c r="M54" s="5"/>
       <c r="N54" s="5"/>
       <c r="O54" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="P54" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="P54" s="7" t="s">
-        <v>279</v>
       </c>
       <c r="Q54" s="5"/>
       <c r="R54" s="5"/>
@@ -5796,28 +5804,28 @@
     </row>
     <row r="55" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D55" s="5">
         <v>2</v>
       </c>
       <c r="E55" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="G55" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="G55" s="5" t="s">
+      <c r="H55" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
@@ -5826,10 +5834,10 @@
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
       <c r="O55" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="P55" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="P55" s="7" t="s">
-        <v>279</v>
       </c>
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
@@ -5845,28 +5853,28 @@
     </row>
     <row r="56" spans="1:27" ht="36" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D56" s="5">
         <v>1</v>
       </c>
       <c r="E56" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="G56" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="H56" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>285</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
@@ -5875,10 +5883,10 @@
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
       <c r="O56" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="P56" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="P56" s="7" t="s">
-        <v>279</v>
       </c>
       <c r="Q56" s="5"/>
       <c r="R56" s="5"/>
@@ -5894,28 +5902,28 @@
     </row>
     <row r="57" spans="1:27" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D57" s="5">
         <v>3</v>
       </c>
       <c r="E57" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="G57" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="H57" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
@@ -5924,10 +5932,10 @@
       <c r="M57" s="5"/>
       <c r="N57" s="5"/>
       <c r="O57" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P57" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q57" s="5"/>
       <c r="R57" s="5"/>
@@ -5943,28 +5951,28 @@
     </row>
     <row r="58" spans="1:27" ht="51" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D58" s="5">
         <v>2</v>
       </c>
       <c r="E58" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="F58" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="G58" s="5" t="s">
+      <c r="H58" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>294</v>
       </c>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
@@ -5973,10 +5981,10 @@
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
       <c r="O58" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P58" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q58" s="5"/>
       <c r="R58" s="5"/>
@@ -5992,28 +6000,28 @@
     </row>
     <row r="59" spans="1:27" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D59" s="5">
         <v>4</v>
       </c>
       <c r="E59" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H59" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
@@ -6022,10 +6030,10 @@
       <c r="M59" s="5"/>
       <c r="N59" s="5"/>
       <c r="O59" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P59" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q59" s="5"/>
       <c r="R59" s="5"/>
@@ -6041,28 +6049,28 @@
     </row>
     <row r="60" spans="1:27" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D60" s="5">
         <v>3</v>
       </c>
       <c r="E60" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="G60" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H60" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>306</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
@@ -6071,10 +6079,10 @@
       <c r="M60" s="5"/>
       <c r="N60" s="5"/>
       <c r="O60" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P60" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q60" s="5"/>
       <c r="R60" s="5"/>
@@ -6090,28 +6098,28 @@
     </row>
     <row r="61" spans="1:27" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D61" s="5">
         <v>2</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F61" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="H61" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>309</v>
       </c>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
@@ -6120,10 +6128,10 @@
       <c r="M61" s="5"/>
       <c r="N61" s="5"/>
       <c r="O61" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P61" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q61" s="5"/>
       <c r="R61" s="5"/>
@@ -6139,29 +6147,29 @@
     </row>
     <row r="62" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="G62" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="H62" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="I62" s="4" t="s">
         <v>315</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>316</v>
       </c>
       <c r="J62" s="5">
         <v>4</v>
@@ -6179,10 +6187,10 @@
         <v>3</v>
       </c>
       <c r="O62" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P62" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Q62" s="5"/>
       <c r="R62" s="5"/>
@@ -6198,42 +6206,42 @@
     </row>
     <row r="63" spans="1:27" ht="126" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="F63" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="F63" s="15" t="s">
+      <c r="G63" s="15" t="s">
         <v>318</v>
-      </c>
-      <c r="G63" s="15" t="s">
-        <v>319</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K63" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="L63" s="14" t="s">
         <v>320</v>
-      </c>
-      <c r="L63" s="14" t="s">
-        <v>321</v>
       </c>
       <c r="M63" s="11"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P63" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q63" s="5"/>
       <c r="R63" s="5"/>

</xml_diff>